<commit_message>
completed with Mech Section and BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryans\Documents\Adinkra_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215889EF-26B1-4EF2-AF58-47CAB6D5BA67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27382C52-BBE6-4170-8E69-AC555E43C496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>https://www.homedepot.com/p/Crown-Bolt-1-4-in-20-x-5-8-in-Phillips-Slotted-Round-Head-Machine-Screws-2-Pack-61018/100337753</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B089S2QDHD/ref=emc_b_5_t?th=1</t>
+  </si>
+  <si>
+    <t>OVERTURE PLA Matte Filament 1.75mm, Matte PLA Roll 1kg Cardboard Spool (2.2lbs), Dimensional Accuracy +/- 0.03 mm, Fit Most FDM Printer (Black)</t>
+  </si>
+  <si>
+    <t>65 g &amp; 21.96m PLA if printed together, else: socket = 14g &amp; 4.80m; ball joint =  16g &amp; 5.32m; magnet housing = 35g &amp; 11.84m. "pla matte" is stronger</t>
   </si>
 </sst>
 </file>
@@ -499,13 +508,13 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="57.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="47.85546875" style="1" customWidth="1"/>
     <col min="3" max="5" width="9.140625" style="1"/>
     <col min="6" max="6" width="71.42578125" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
@@ -590,7 +599,7 @@
         <f t="shared" si="0"/>
         <v>1.18</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -611,7 +620,7 @@
         <f t="shared" si="0"/>
         <v>1.28</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -632,7 +641,7 @@
         <f t="shared" si="0"/>
         <v>1.1100000000000001</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -653,15 +662,29 @@
         <f t="shared" si="0"/>
         <v>0.68</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D8" s="2"/>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>19.989999999999998</v>
+      </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>19.989999999999998</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -839,18 +862,23 @@
       <c r="D33" s="2"/>
       <c r="E33" s="2">
         <f>SUM(E2:E32)</f>
-        <v>14.419999999999998</v>
+        <v>34.409999999999997</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{462AC750-D4FC-4879-BB32-385EFB5C966E}"/>
     <hyperlink ref="F3" r:id="rId2" xr:uid="{F8204AB4-19B6-413C-AC10-C1F76CC764DB}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{B92E143F-4613-4886-8660-E96982FA4F69}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{46C212E6-E982-4B8A-BE96-E9C4E6C02EC2}"/>
+    <hyperlink ref="F6" r:id="rId5" location="overlay" xr:uid="{1D1229D9-3A1C-4255-B5D0-3DC90EF88AAF}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{50451D9C-0998-429E-B234-FDC5FE2E2B88}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{A0AEBB5B-870E-4450-9DF0-80E8102F042E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cut outs added to magnet housing. BOM updated
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryans\Documents\Adinkra_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27382C52-BBE6-4170-8E69-AC555E43C496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC78D01-C79C-4C5B-ACE4-2423CA0BE6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,7 +114,7 @@
     <t>OVERTURE PLA Matte Filament 1.75mm, Matte PLA Roll 1kg Cardboard Spool (2.2lbs), Dimensional Accuracy +/- 0.03 mm, Fit Most FDM Printer (Black)</t>
   </si>
   <si>
-    <t>65 g &amp; 21.96m PLA if printed together, else: socket = 14g &amp; 4.80m; ball joint =  16g &amp; 5.32m; magnet housing = 35g &amp; 11.84m. "pla matte" is stronger</t>
+    <t>65 g &amp; 21.82m PLA if printed together, else: socket = 14g &amp; 4.80m; ball joint =  16g &amp; 5.32m; magnet housing = 35g &amp; 11.61m. "pla matte" is stronger</t>
   </si>
 </sst>
 </file>
@@ -508,7 +508,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>